<commit_message>
VMP vs ML with fading
</commit_message>
<xml_diff>
--- a/IDA2015/PreliminaryExperiments/Fading.xlsx
+++ b/IDA2015/PreliminaryExperiments/Fading.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VMPvsML" sheetId="2" r:id="rId1"/>
+    <sheet name="VMP" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="16">
   <si>
     <t xml:space="preserve">WindowSize </t>
   </si>
@@ -56,12 +57,27 @@
   <si>
     <t>Var B with 0.5 MAR</t>
   </si>
+  <si>
+    <t>VMP @ DIFFERENT FADING FACTORS</t>
+  </si>
+  <si>
+    <t>ML @ DIFFERENT FADING FACTORS</t>
+  </si>
+  <si>
+    <t>DIFFERENCES</t>
+  </si>
+  <si>
+    <t>POSITIVE IS GOOD FOR VMP OVERALL(except at the beginning)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +101,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -100,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,8 +132,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -149,16 +182,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -178,6 +273,31 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -197,6 +317,31 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,10 +671,2594 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.999</v>
+      </c>
+      <c r="E3">
+        <v>0.99</v>
+      </c>
+      <c r="F3">
+        <v>0.9</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
+      </c>
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+      <c r="I3">
+        <v>0.6</v>
+      </c>
+      <c r="J3">
+        <v>0.5</v>
+      </c>
+      <c r="K3">
+        <v>0.4</v>
+      </c>
+      <c r="L3">
+        <v>0.3</v>
+      </c>
+      <c r="M3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>8.0121239229503107</v>
+      </c>
+      <c r="C4">
+        <v>8.0031987780625098</v>
+      </c>
+      <c r="D4">
+        <v>7.9396244306663402</v>
+      </c>
+      <c r="E4">
+        <v>7.8000740585204804</v>
+      </c>
+      <c r="F4">
+        <v>7.0531333622822601</v>
+      </c>
+      <c r="G4">
+        <v>6.8894801899536802</v>
+      </c>
+      <c r="H4">
+        <v>6.88051167044366</v>
+      </c>
+      <c r="I4">
+        <v>6.7610380569257504</v>
+      </c>
+      <c r="J4">
+        <v>6.5143196191097399</v>
+      </c>
+      <c r="K4">
+        <v>6.3334696292653101</v>
+      </c>
+      <c r="L4">
+        <v>6.4560598733062697</v>
+      </c>
+      <c r="M4">
+        <v>6.3464322042218999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>8.0129448112974995</v>
+      </c>
+      <c r="C5">
+        <v>8.0086216619531694</v>
+      </c>
+      <c r="D5">
+        <v>7.9625442759019496</v>
+      </c>
+      <c r="E5">
+        <v>7.8942809466319401</v>
+      </c>
+      <c r="F5">
+        <v>7.3450914799290299</v>
+      </c>
+      <c r="G5">
+        <v>7.0287008147214198</v>
+      </c>
+      <c r="H5">
+        <v>6.8955453191758203</v>
+      </c>
+      <c r="I5">
+        <v>6.8693798405794002</v>
+      </c>
+      <c r="J5">
+        <v>6.8644024074440297</v>
+      </c>
+      <c r="K5">
+        <v>6.6875502616190197</v>
+      </c>
+      <c r="L5">
+        <v>6.12097512035304</v>
+      </c>
+      <c r="M5">
+        <v>5.44888016616183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>8.0155291600518108</v>
+      </c>
+      <c r="C6">
+        <v>8.0145919182421501</v>
+      </c>
+      <c r="D6">
+        <v>8.0051427925046994</v>
+      </c>
+      <c r="E6">
+        <v>7.9393499135033903</v>
+      </c>
+      <c r="F6">
+        <v>7.7916514507113099</v>
+      </c>
+      <c r="G6">
+        <v>7.6303374316832002</v>
+      </c>
+      <c r="H6">
+        <v>7.5199502940380301</v>
+      </c>
+      <c r="I6">
+        <v>7.4334362879878801</v>
+      </c>
+      <c r="J6">
+        <v>7.3592666401179896</v>
+      </c>
+      <c r="K6">
+        <v>7.29473530351504</v>
+      </c>
+      <c r="L6">
+        <v>7.2407026688400897</v>
+      </c>
+      <c r="M6">
+        <v>7.1988672399099096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>8.0161624427534104</v>
+      </c>
+      <c r="C7">
+        <v>8.0160654015890191</v>
+      </c>
+      <c r="D7">
+        <v>8.01518029198356</v>
+      </c>
+      <c r="E7">
+        <v>8.0053277617997196</v>
+      </c>
+      <c r="F7">
+        <v>7.9358265574018301</v>
+      </c>
+      <c r="G7">
+        <v>7.9184794931998299</v>
+      </c>
+      <c r="H7">
+        <v>7.9012166281168801</v>
+      </c>
+      <c r="I7">
+        <v>7.8762479847256701</v>
+      </c>
+      <c r="J7">
+        <v>7.84245447674716</v>
+      </c>
+      <c r="K7">
+        <v>7.8019241539761097</v>
+      </c>
+      <c r="L7">
+        <v>7.7581061331786501</v>
+      </c>
+      <c r="M7">
+        <v>7.7143941932238702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>8.0171273029509802</v>
+      </c>
+      <c r="C8">
+        <v>8.0171167777488002</v>
+      </c>
+      <c r="D8">
+        <v>8.0170218733221503</v>
+      </c>
+      <c r="E8">
+        <v>8.01605520640795</v>
+      </c>
+      <c r="F8">
+        <v>8.0046304960272394</v>
+      </c>
+      <c r="G8">
+        <v>7.9886190020571304</v>
+      </c>
+      <c r="H8">
+        <v>7.9706359546334697</v>
+      </c>
+      <c r="I8">
+        <v>7.9527659937986801</v>
+      </c>
+      <c r="J8">
+        <v>7.9366194882686401</v>
+      </c>
+      <c r="K8">
+        <v>7.92286797092485</v>
+      </c>
+      <c r="L8">
+        <v>7.9114499785195296</v>
+      </c>
+      <c r="M8">
+        <v>7.9019756189379402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.999</v>
+      </c>
+      <c r="E10">
+        <v>0.99</v>
+      </c>
+      <c r="F10">
+        <v>0.9</v>
+      </c>
+      <c r="G10">
+        <v>0.8</v>
+      </c>
+      <c r="H10">
+        <v>0.7</v>
+      </c>
+      <c r="I10">
+        <v>0.6</v>
+      </c>
+      <c r="J10">
+        <v>0.5</v>
+      </c>
+      <c r="K10">
+        <v>0.4</v>
+      </c>
+      <c r="L10">
+        <v>0.3</v>
+      </c>
+      <c r="M10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>8.0173634558182201</v>
+      </c>
+      <c r="C11">
+        <v>8.0064571985357098</v>
+      </c>
+      <c r="D11">
+        <v>7.9406171534180796</v>
+      </c>
+      <c r="E11">
+        <v>7.8163951797139202</v>
+      </c>
+      <c r="F11">
+        <v>7.0690724416484896</v>
+      </c>
+      <c r="G11">
+        <v>6.5061055669308097</v>
+      </c>
+      <c r="H11">
+        <v>6.0365588764655502</v>
+      </c>
+      <c r="I11">
+        <v>5.6763121704986901</v>
+      </c>
+      <c r="J11">
+        <v>5.4205711695756396</v>
+      </c>
+      <c r="K11">
+        <v>5.2555274006412898</v>
+      </c>
+      <c r="L11">
+        <v>5.17276612852414</v>
+      </c>
+      <c r="M11">
+        <v>5.1699383292516696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>8.0173634558182307</v>
+      </c>
+      <c r="C12">
+        <v>8.0121389991512508</v>
+      </c>
+      <c r="D12">
+        <v>7.9633223261020101</v>
+      </c>
+      <c r="E12">
+        <v>7.9042079529392497</v>
+      </c>
+      <c r="F12">
+        <v>7.3973373087988001</v>
+      </c>
+      <c r="G12">
+        <v>7.0258794876498998</v>
+      </c>
+      <c r="H12">
+        <v>6.6685272073196202</v>
+      </c>
+      <c r="I12">
+        <v>6.3098589958996198</v>
+      </c>
+      <c r="J12">
+        <v>5.9549384690475904</v>
+      </c>
+      <c r="K12">
+        <v>5.6151368535958097</v>
+      </c>
+      <c r="L12">
+        <v>5.2952668583419999</v>
+      </c>
+      <c r="M12">
+        <v>4.9926871065458096</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>8.0173634558182201</v>
+      </c>
+      <c r="C13">
+        <v>8.0163624824051105</v>
+      </c>
+      <c r="D13">
+        <v>8.0064537300120797</v>
+      </c>
+      <c r="E13">
+        <v>7.9405076512955803</v>
+      </c>
+      <c r="F13">
+        <v>7.8128873262275498</v>
+      </c>
+      <c r="G13">
+        <v>7.6629330497561501</v>
+      </c>
+      <c r="H13">
+        <v>7.5636325480224897</v>
+      </c>
+      <c r="I13">
+        <v>7.4823607514177004</v>
+      </c>
+      <c r="J13">
+        <v>7.4055463934751602</v>
+      </c>
+      <c r="K13">
+        <v>7.3318782966229303</v>
+      </c>
+      <c r="L13">
+        <v>7.26612452823385</v>
+      </c>
+      <c r="M13">
+        <v>7.2135428913783999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>8.0173634558182307</v>
+      </c>
+      <c r="C14">
+        <v>8.01726320631089</v>
+      </c>
+      <c r="D14">
+        <v>8.0163498864552007</v>
+      </c>
+      <c r="E14">
+        <v>8.0062788819285604</v>
+      </c>
+      <c r="F14">
+        <v>7.9364545301694696</v>
+      </c>
+      <c r="G14">
+        <v>7.9203983486946496</v>
+      </c>
+      <c r="H14">
+        <v>7.9054008408357701</v>
+      </c>
+      <c r="I14">
+        <v>7.8831602460112498</v>
+      </c>
+      <c r="J14">
+        <v>7.8520333356389296</v>
+      </c>
+      <c r="K14">
+        <v>7.8133293175046399</v>
+      </c>
+      <c r="L14">
+        <v>7.7697317774917298</v>
+      </c>
+      <c r="M14">
+        <v>7.7242044944844297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>1000</v>
+      </c>
+      <c r="B15">
+        <v>8.0173634558182307</v>
+      </c>
+      <c r="C15">
+        <v>8.01726320631089</v>
+      </c>
+      <c r="D15">
+        <v>8.0163498864552007</v>
+      </c>
+      <c r="E15">
+        <v>8.0062788819285604</v>
+      </c>
+      <c r="F15">
+        <v>7.9364545301694696</v>
+      </c>
+      <c r="G15">
+        <v>7.9203983486946496</v>
+      </c>
+      <c r="H15">
+        <v>7.9054008408357701</v>
+      </c>
+      <c r="I15">
+        <v>7.8831602460112498</v>
+      </c>
+      <c r="J15">
+        <v>7.8520333356389296</v>
+      </c>
+      <c r="K15">
+        <v>7.8133293175046399</v>
+      </c>
+      <c r="L15">
+        <v>7.7697317774917298</v>
+      </c>
+      <c r="M15">
+        <v>7.7242044944844297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7">
+        <f>B4-B11</f>
+        <v>-5.2395328679093467E-3</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" ref="C17:M17" si="0">C4-C11</f>
+        <v>-3.2584204732000188E-3</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>-9.927227517394499E-4</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.6321121193439758E-2</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.5939079366229514E-2</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.38337462302287051</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.84395279397810974</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0847258864270604</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0937484495341003</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0779422286240203</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2832937447821298</v>
+      </c>
+      <c r="M17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.1764938749702303</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="7">
+        <f>B5-B12</f>
+        <v>-4.418644520731263E-3</v>
+      </c>
+      <c r="C18" s="7">
+        <f>C5-C12</f>
+        <v>-3.5173371980814494E-3</v>
+      </c>
+      <c r="D18" s="7">
+        <f>D5-D12</f>
+        <v>-7.780502000604983E-4</v>
+      </c>
+      <c r="E18" s="7">
+        <f>E5-E12</f>
+        <v>-9.9270063073095827E-3</v>
+      </c>
+      <c r="F18" s="7">
+        <f>F5-F12</f>
+        <v>-5.224582886977025E-2</v>
+      </c>
+      <c r="G18" s="7">
+        <f>G5-G12</f>
+        <v>2.8213270715200522E-3</v>
+      </c>
+      <c r="H18" s="7">
+        <f>H5-H12</f>
+        <v>0.22701811185620002</v>
+      </c>
+      <c r="I18" s="7">
+        <f>I5-I12</f>
+        <v>0.55952084467978036</v>
+      </c>
+      <c r="J18" s="7">
+        <f>J5-J12</f>
+        <v>0.90946393839643935</v>
+      </c>
+      <c r="K18" s="7">
+        <f>K5-K12</f>
+        <v>1.0724134080232099</v>
+      </c>
+      <c r="L18" s="7">
+        <f>L5-L12</f>
+        <v>0.82570826201104008</v>
+      </c>
+      <c r="M18" s="7">
+        <f>M5-M12</f>
+        <v>0.45619305961602041</v>
+      </c>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" s="7">
+        <f>B6-B13</f>
+        <v>-1.8342957664092552E-3</v>
+      </c>
+      <c r="C19" s="7">
+        <f>C6-C13</f>
+        <v>-1.7705641629603974E-3</v>
+      </c>
+      <c r="D19" s="7">
+        <f>D6-D13</f>
+        <v>-1.3109375073803164E-3</v>
+      </c>
+      <c r="E19" s="7">
+        <f>E6-E13</f>
+        <v>-1.1577377921900833E-3</v>
+      </c>
+      <c r="F19" s="7">
+        <f>F6-F13</f>
+        <v>-2.1235875516239844E-2</v>
+      </c>
+      <c r="G19" s="7">
+        <f>G6-G13</f>
+        <v>-3.2595618072949861E-2</v>
+      </c>
+      <c r="H19" s="7">
+        <f>H6-H13</f>
+        <v>-4.3682253984459685E-2</v>
+      </c>
+      <c r="I19" s="7">
+        <f>I6-I13</f>
+        <v>-4.8924463429820264E-2</v>
+      </c>
+      <c r="J19" s="7">
+        <f>J6-J13</f>
+        <v>-4.6279753357170605E-2</v>
+      </c>
+      <c r="K19" s="7">
+        <f>K6-K13</f>
+        <v>-3.7142993107890376E-2</v>
+      </c>
+      <c r="L19" s="7">
+        <f>L6-L13</f>
+        <v>-2.5421859393760293E-2</v>
+      </c>
+      <c r="M19" s="7">
+        <f>M6-M13</f>
+        <v>-1.4675651468490258E-2</v>
+      </c>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="B20" s="7">
+        <f>B7-B14</f>
+        <v>-1.2010130648203443E-3</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" ref="C20:M20" si="1">C7-C14</f>
+        <v>-1.1978047218708099E-3</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.169594471640778E-3</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="1"/>
+        <v>-9.5112012884079888E-4</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="1"/>
+        <v>-6.2797276763948418E-4</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.9188554948197378E-3</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="1"/>
+        <v>-4.1842127188900236E-3</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="1"/>
+        <v>-6.9122612855796461E-3</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="1"/>
+        <v>-9.5788588917695705E-3</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.140516352853016E-2</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.1625644313079775E-2</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" si="1"/>
+        <v>-9.8103012605594841E-3</v>
+      </c>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="7">
+        <f t="shared" ref="B21:M21" si="2">B8-B15</f>
+        <v>-2.3615286725053863E-4</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="2"/>
+        <v>-1.4642856208979538E-4</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="2"/>
+        <v>6.7198686694958099E-4</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="2"/>
+        <v>9.7763244793895865E-3</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="2"/>
+        <v>6.817596585776986E-2</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="2"/>
+        <v>6.8220653362480732E-2</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="2"/>
+        <v>6.523511379769964E-2</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="2"/>
+        <v>6.9605747787430339E-2</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="2"/>
+        <v>8.4586152629710476E-2</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="2"/>
+        <v>0.10953865342021007</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" si="2"/>
+        <v>0.14171820102779975</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" si="2"/>
+        <v>0.17777112445351051</v>
+      </c>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+    </row>
+    <row r="22" spans="1:18" ht="16" thickBot="1">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+    </row>
+    <row r="23" spans="1:18" ht="16" thickTop="1">
+      <c r="A23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0.999</v>
+      </c>
+      <c r="F24">
+        <v>0.99</v>
+      </c>
+      <c r="G24">
+        <v>0.9</v>
+      </c>
+      <c r="H24">
+        <v>0.8</v>
+      </c>
+      <c r="I24">
+        <v>0.7</v>
+      </c>
+      <c r="J24">
+        <v>0.6</v>
+      </c>
+      <c r="K24">
+        <v>0.5</v>
+      </c>
+      <c r="L24">
+        <v>0.4</v>
+      </c>
+      <c r="M24">
+        <v>0.3</v>
+      </c>
+      <c r="N24">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>7.2996155077084302</v>
+      </c>
+      <c r="C25">
+        <v>7.06433091075679</v>
+      </c>
+      <c r="D25">
+        <v>4.58917904262288</v>
+      </c>
+      <c r="E25">
+        <v>-0.81669802664189795</v>
+      </c>
+      <c r="F25">
+        <v>-0.81759153017581998</v>
+      </c>
+      <c r="G25">
+        <v>-0.79056030839072799</v>
+      </c>
+      <c r="H25">
+        <v>-0.80004960140728898</v>
+      </c>
+      <c r="I25">
+        <v>-0.83279269144110801</v>
+      </c>
+      <c r="J25">
+        <v>-0.87599645254285097</v>
+      </c>
+      <c r="K25">
+        <v>-0.97415958110404</v>
+      </c>
+      <c r="L25">
+        <v>-1.0773049459689199</v>
+      </c>
+      <c r="M25">
+        <v>-1.0950362168144401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>0.47534157521737003</v>
+      </c>
+      <c r="C26">
+        <v>0.45747087851835799</v>
+      </c>
+      <c r="D26">
+        <v>0.26331719573553602</v>
+      </c>
+      <c r="E26">
+        <v>-0.74679280115009095</v>
+      </c>
+      <c r="F26">
+        <v>-0.86191352345017302</v>
+      </c>
+      <c r="G26">
+        <v>-0.81894115933418798</v>
+      </c>
+      <c r="H26">
+        <v>-0.80505836554077603</v>
+      </c>
+      <c r="I26">
+        <v>-0.80848107096994304</v>
+      </c>
+      <c r="J26">
+        <v>-0.82086891126574302</v>
+      </c>
+      <c r="K26">
+        <v>-0.84060754452978603</v>
+      </c>
+      <c r="L26">
+        <v>-0.86170964511699999</v>
+      </c>
+      <c r="M26">
+        <v>-0.87351504574208405</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>-1.3209082813572199</v>
+      </c>
+      <c r="C27">
+        <v>-1.3198607376881699</v>
+      </c>
+      <c r="D27">
+        <v>-1.3099604625098999</v>
+      </c>
+      <c r="E27">
+        <v>-1.1876981084171401</v>
+      </c>
+      <c r="F27">
+        <v>-0.90174379857509601</v>
+      </c>
+      <c r="G27">
+        <v>-0.89300953256882398</v>
+      </c>
+      <c r="H27">
+        <v>-0.88434113933530101</v>
+      </c>
+      <c r="I27">
+        <v>-0.87274701728259396</v>
+      </c>
+      <c r="J27">
+        <v>-0.85902023872876698</v>
+      </c>
+      <c r="K27">
+        <v>-0.84701842992915899</v>
+      </c>
+      <c r="L27">
+        <v>-0.84647203731134102</v>
+      </c>
+      <c r="M27">
+        <v>-0.86466966995556704</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28">
+        <v>100</v>
+      </c>
+      <c r="B28">
+        <v>-0.83745429720667097</v>
+      </c>
+      <c r="C28">
+        <v>-0.83747065365011997</v>
+      </c>
+      <c r="D28">
+        <v>-0.83761567821036897</v>
+      </c>
+      <c r="E28">
+        <v>-0.83904960941296702</v>
+      </c>
+      <c r="F28">
+        <v>-0.85437570633723403</v>
+      </c>
+      <c r="G28">
+        <v>-0.87444362379861196</v>
+      </c>
+      <c r="H28">
+        <v>-0.889264217107264</v>
+      </c>
+      <c r="I28">
+        <v>-0.89970919069233402</v>
+      </c>
+      <c r="J28">
+        <v>-0.90783181745791397</v>
+      </c>
+      <c r="K28">
+        <v>-0.91635075275574696</v>
+      </c>
+      <c r="L28">
+        <v>-0.92686402922989397</v>
+      </c>
+      <c r="M28">
+        <v>-0.938931015592819</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>-0.862961577700329</v>
+      </c>
+      <c r="C29">
+        <v>-0.86296277296495105</v>
+      </c>
+      <c r="D29">
+        <v>-0.86297353815755395</v>
+      </c>
+      <c r="E29">
+        <v>-0.86308195779649099</v>
+      </c>
+      <c r="F29">
+        <v>-0.86422992908552498</v>
+      </c>
+      <c r="G29">
+        <v>-0.865621721560489</v>
+      </c>
+      <c r="H29">
+        <v>-0.86710847366632005</v>
+      </c>
+      <c r="I29">
+        <v>-0.868978423071326</v>
+      </c>
+      <c r="J29">
+        <v>-0.87227653810618</v>
+      </c>
+      <c r="K29">
+        <v>-0.87703674148849298</v>
+      </c>
+      <c r="L29">
+        <v>-0.88391729751420001</v>
+      </c>
+      <c r="M29">
+        <v>-0.89384926363224804</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D31">
+        <v>0.999</v>
+      </c>
+      <c r="E31">
+        <v>0.99</v>
+      </c>
+      <c r="F31">
+        <v>0.9</v>
+      </c>
+      <c r="G31">
+        <v>0.8</v>
+      </c>
+      <c r="H31">
+        <v>0.7</v>
+      </c>
+      <c r="I31">
+        <v>0.6</v>
+      </c>
+      <c r="J31">
+        <v>0.5</v>
+      </c>
+      <c r="K31">
+        <v>0.4</v>
+      </c>
+      <c r="L31">
+        <v>0.3</v>
+      </c>
+      <c r="M31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="11">
+        <v>-8.3333523932117794E-5</v>
+      </c>
+      <c r="C32" s="11">
+        <v>-8.3552399525793202E-5</v>
+      </c>
+      <c r="D32" s="11">
+        <v>-8.6283371845775796E-5</v>
+      </c>
+      <c r="E32" s="11">
+        <v>-8.2861282865675305E-5</v>
+      </c>
+      <c r="F32" s="11">
+        <v>-5.5716424380759599E-5</v>
+      </c>
+      <c r="G32" s="11">
+        <v>-4.9254949814149498E-5</v>
+      </c>
+      <c r="H32" s="11">
+        <v>-5.8832891976867302E-5</v>
+      </c>
+      <c r="I32" s="11">
+        <v>-6.8581958171616499E-5</v>
+      </c>
+      <c r="J32" s="11">
+        <v>-7.2843265616661797E-5</v>
+      </c>
+      <c r="K32" s="11">
+        <v>-6.9944357906068206E-5</v>
+      </c>
+      <c r="L32" s="11">
+        <v>-6.0125497336990402E-5</v>
+      </c>
+      <c r="M32" s="11">
+        <v>-4.45281170459036E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="11">
+        <v>-1.6681863629364099E-4</v>
+      </c>
+      <c r="C33" s="11">
+        <v>-1.6702933725573201E-4</v>
+      </c>
+      <c r="D33" s="11">
+        <v>-1.6958085416409599E-4</v>
+      </c>
+      <c r="E33" s="11">
+        <v>-1.71662155940797E-4</v>
+      </c>
+      <c r="F33" s="11">
+        <v>-1.49535675184001E-4</v>
+      </c>
+      <c r="G33" s="11">
+        <v>-1.1534328588589099E-4</v>
+      </c>
+      <c r="H33" s="11">
+        <v>-1.08215951347589E-4</v>
+      </c>
+      <c r="I33" s="11">
+        <v>-1.1993926347477199E-4</v>
+      </c>
+      <c r="J33" s="11">
+        <v>-1.41846511088896E-4</v>
+      </c>
+      <c r="K33" s="11">
+        <v>-1.6749774827569299E-4</v>
+      </c>
+      <c r="L33" s="11">
+        <v>-1.9163838699065501E-4</v>
+      </c>
+      <c r="M33" s="11">
+        <v>-2.0888587352538399E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34" s="11">
+        <v>-8.4020671708269403E-4</v>
+      </c>
+      <c r="C34" s="11">
+        <v>-8.40413300644979E-4</v>
+      </c>
+      <c r="D34" s="11">
+        <v>-8.4242414553949098E-4</v>
+      </c>
+      <c r="E34" s="11">
+        <v>-8.7007415485178198E-4</v>
+      </c>
+      <c r="F34" s="11">
+        <v>-8.2988731413960405E-4</v>
+      </c>
+      <c r="G34" s="11">
+        <v>-8.2440783779648397E-4</v>
+      </c>
+      <c r="H34" s="11">
+        <v>-7.9097389464827196E-4</v>
+      </c>
+      <c r="I34" s="11">
+        <v>-7.2135148150229101E-4</v>
+      </c>
+      <c r="J34" s="11">
+        <v>-6.3350036458344097E-4</v>
+      </c>
+      <c r="K34" s="11">
+        <v>-5.4094313923358495E-4</v>
+      </c>
+      <c r="L34" s="11">
+        <v>-4.50916754603805E-4</v>
+      </c>
+      <c r="M34" s="11">
+        <v>-3.6651065228451802E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <v>-9.1571426704323208E-3</v>
+      </c>
+      <c r="C35">
+        <v>-9.1573690115664894E-3</v>
+      </c>
+      <c r="D35">
+        <v>-9.1594227090762096E-3</v>
+      </c>
+      <c r="E35">
+        <v>-9.1815874634615293E-3</v>
+      </c>
+      <c r="F35">
+        <v>-9.4826627494157805E-3</v>
+      </c>
+      <c r="G35">
+        <v>-9.6198207228113102E-3</v>
+      </c>
+      <c r="H35">
+        <v>-9.5208160641185799E-3</v>
+      </c>
+      <c r="I35">
+        <v>-9.3404766513829306E-3</v>
+      </c>
+      <c r="J35">
+        <v>-9.1725321272768598E-3</v>
+      </c>
+      <c r="K35">
+        <v>-9.05767767644205E-3</v>
+      </c>
+      <c r="L35">
+        <v>-9.0088542365525104E-3</v>
+      </c>
+      <c r="M35">
+        <v>-9.02623374547162E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36">
+        <v>1000</v>
+      </c>
+      <c r="B36">
+        <v>-0.90376867720365905</v>
+      </c>
+      <c r="C36">
+        <v>-0.90377318580227395</v>
+      </c>
+      <c r="D36">
+        <v>-0.90381378770087395</v>
+      </c>
+      <c r="E36">
+        <v>-0.90422224077853897</v>
+      </c>
+      <c r="F36">
+        <v>-0.90855863307655704</v>
+      </c>
+      <c r="G36">
+        <v>-0.91395966997354705</v>
+      </c>
+      <c r="H36">
+        <v>-0.92006251832926</v>
+      </c>
+      <c r="I36">
+        <v>-0.92695283057450095</v>
+      </c>
+      <c r="J36">
+        <v>-0.93466344251740796</v>
+      </c>
+      <c r="K36">
+        <v>-0.94315619904727999</v>
+      </c>
+      <c r="L36">
+        <v>-0.95233917485680297</v>
+      </c>
+      <c r="M36">
+        <v>-0.96209054540524896</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="7">
+        <f>B25-B32</f>
+        <v>7.2996988412323622</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" ref="C38:M38" si="3">C25-C32</f>
+        <v>7.0644144631563162</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="3"/>
+        <v>4.5892653259947256</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.81661516535903222</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.81753581375143924</v>
+      </c>
+      <c r="G38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.79051105344091388</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.79999076851531215</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.8327241094829364</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.87592360927723434</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.97408963674613391</v>
+      </c>
+      <c r="L38" s="7">
+        <f t="shared" si="3"/>
+        <v>-1.077244820471583</v>
+      </c>
+      <c r="M38" s="7">
+        <f t="shared" si="3"/>
+        <v>-1.0949916886973943</v>
+      </c>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="7">
+        <f t="shared" ref="B39:M42" si="4">B26-B33</f>
+        <v>0.47550839385366367</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" si="4"/>
+        <v>0.4576379078556137</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="4"/>
+        <v>0.2634867765897001</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.74662113899415017</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.86176398777498897</v>
+      </c>
+      <c r="G39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.81882581604830207</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.80495014958942845</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.80836113170646828</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.82072706475465407</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.8404400467815103</v>
+      </c>
+      <c r="L39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.86151800673000933</v>
+      </c>
+      <c r="M39" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.87330615986855864</v>
+      </c>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40" s="7">
+        <f t="shared" si="4"/>
+        <v>-1.3200680746401372</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" si="4"/>
+        <v>-1.3190203243875249</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="4"/>
+        <v>-1.3091180383643604</v>
+      </c>
+      <c r="E40" s="7">
+        <f t="shared" si="4"/>
+        <v>-1.1868280342622883</v>
+      </c>
+      <c r="F40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.90091391126095643</v>
+      </c>
+      <c r="G40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.89218512473102751</v>
+      </c>
+      <c r="H40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.88355016544065279</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.87202566580109164</v>
+      </c>
+      <c r="J40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.85838673836418355</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.8464774867899254</v>
+      </c>
+      <c r="L40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.84602112055673717</v>
+      </c>
+      <c r="M40" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.8643031593032825</v>
+      </c>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41">
+        <v>100</v>
+      </c>
+      <c r="B41" s="7">
+        <f>B28-B35</f>
+        <v>-0.82829715453623864</v>
+      </c>
+      <c r="C41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.82831328463855347</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.82845625550129276</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.82986802194950549</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.84489304358781825</v>
+      </c>
+      <c r="G41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.86482380307580065</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.87974340104314541</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.89036871404095108</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.8986592853306371</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.9072930750793049</v>
+      </c>
+      <c r="L41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.91785517499334146</v>
+      </c>
+      <c r="M41" s="7">
+        <f t="shared" si="4"/>
+        <v>-0.92990478184734737</v>
+      </c>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42">
+        <v>1000</v>
+      </c>
+      <c r="B42" s="7">
+        <f t="shared" si="4"/>
+        <v>4.0807099503330058E-2</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" si="4"/>
+        <v>4.0810412837322896E-2</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="4"/>
+        <v>4.0840249543319995E-2</v>
+      </c>
+      <c r="E42" s="7">
+        <f t="shared" si="4"/>
+        <v>4.1140282982047971E-2</v>
+      </c>
+      <c r="F42" s="7">
+        <f t="shared" si="4"/>
+        <v>4.4328703991032059E-2</v>
+      </c>
+      <c r="G42" s="7">
+        <f t="shared" si="4"/>
+        <v>4.8337948413058052E-2</v>
+      </c>
+      <c r="H42" s="7">
+        <f t="shared" si="4"/>
+        <v>5.2954044662939959E-2</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="4"/>
+        <v>5.7974407503174952E-2</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="4"/>
+        <v>6.2386904411227961E-2</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="4"/>
+        <v>6.6119457558787009E-2</v>
+      </c>
+      <c r="L42" s="7">
+        <f t="shared" si="4"/>
+        <v>6.8421877342602966E-2</v>
+      </c>
+      <c r="M42" s="7">
+        <f t="shared" si="4"/>
+        <v>6.8241281773000928E-2</v>
+      </c>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+    </row>
+    <row r="43" spans="1:18" ht="16" thickBot="1">
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+    </row>
+    <row r="44" spans="1:18" ht="16" thickTop="1">
+      <c r="A44" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D45">
+        <v>0.999</v>
+      </c>
+      <c r="E45">
+        <v>0.99</v>
+      </c>
+      <c r="F45">
+        <v>0.9</v>
+      </c>
+      <c r="G45">
+        <v>0.8</v>
+      </c>
+      <c r="H45">
+        <v>0.7</v>
+      </c>
+      <c r="I45">
+        <v>0.6</v>
+      </c>
+      <c r="J45">
+        <v>0.5</v>
+      </c>
+      <c r="K45">
+        <v>0.4</v>
+      </c>
+      <c r="L45">
+        <v>0.3</v>
+      </c>
+      <c r="M45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>0.153268079571965</v>
+      </c>
+      <c r="C46">
+        <v>0.17922630340731199</v>
+      </c>
+      <c r="D46">
+        <v>0.47263819024463299</v>
+      </c>
+      <c r="E46">
+        <v>1.12736388936475</v>
+      </c>
+      <c r="F46">
+        <v>1.1623914211183599</v>
+      </c>
+      <c r="G46">
+        <v>1.1762674098297601</v>
+      </c>
+      <c r="H46">
+        <v>1.1896108843088899</v>
+      </c>
+      <c r="I46">
+        <v>1.2048459367127</v>
+      </c>
+      <c r="J46">
+        <v>1.2207259222626099</v>
+      </c>
+      <c r="K46">
+        <v>1.2461301961542699</v>
+      </c>
+      <c r="L46">
+        <v>1.27183742921145</v>
+      </c>
+      <c r="M46">
+        <v>1.27791990726009</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>0.96780126010886303</v>
+      </c>
+      <c r="C47">
+        <v>0.96941451102615095</v>
+      </c>
+      <c r="D47">
+        <v>0.99229698282311496</v>
+      </c>
+      <c r="E47">
+        <v>1.11601833586191</v>
+      </c>
+      <c r="F47">
+        <v>1.1530205813939001</v>
+      </c>
+      <c r="G47">
+        <v>1.1610961304520799</v>
+      </c>
+      <c r="H47">
+        <v>1.16801100685092</v>
+      </c>
+      <c r="I47">
+        <v>1.17513746129124</v>
+      </c>
+      <c r="J47">
+        <v>1.18216521420816</v>
+      </c>
+      <c r="K47">
+        <v>1.1892298363621301</v>
+      </c>
+      <c r="L47">
+        <v>1.19560009852848</v>
+      </c>
+      <c r="M47">
+        <v>1.1993696050184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>1.18064359607686</v>
+      </c>
+      <c r="C48">
+        <v>1.18056191033501</v>
+      </c>
+      <c r="D48">
+        <v>1.1797824591097199</v>
+      </c>
+      <c r="E48">
+        <v>1.16719389748893</v>
+      </c>
+      <c r="F48">
+        <v>1.13825944414003</v>
+      </c>
+      <c r="G48">
+        <v>1.1438783660740599</v>
+      </c>
+      <c r="H48">
+        <v>1.1482338778511301</v>
+      </c>
+      <c r="I48">
+        <v>1.15080303116746</v>
+      </c>
+      <c r="J48">
+        <v>1.1519033643785399</v>
+      </c>
+      <c r="K48">
+        <v>1.15223704906388</v>
+      </c>
+      <c r="L48">
+        <v>1.15330793442704</v>
+      </c>
+      <c r="M48">
+        <v>1.1563940319764701</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49">
+        <v>100</v>
+      </c>
+      <c r="B49">
+        <v>1.1240089760276</v>
+      </c>
+      <c r="C49">
+        <v>1.1240109960968601</v>
+      </c>
+      <c r="D49">
+        <v>1.1240289897500699</v>
+      </c>
+      <c r="E49">
+        <v>1.1242144323834999</v>
+      </c>
+      <c r="F49">
+        <v>1.12718517938869</v>
+      </c>
+      <c r="G49">
+        <v>1.1301688702075099</v>
+      </c>
+      <c r="H49">
+        <v>1.1324599786174501</v>
+      </c>
+      <c r="I49">
+        <v>1.1342429335286299</v>
+      </c>
+      <c r="J49">
+        <v>1.1357709964181899</v>
+      </c>
+      <c r="K49">
+        <v>1.1373901139195799</v>
+      </c>
+      <c r="L49">
+        <v>1.1393291694833201</v>
+      </c>
+      <c r="M49">
+        <v>1.14156186468461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50">
+        <v>1000</v>
+      </c>
+      <c r="B50">
+        <v>1.1268282796543101</v>
+      </c>
+      <c r="C50">
+        <v>1.12682846981048</v>
+      </c>
+      <c r="D50">
+        <v>1.12683018315397</v>
+      </c>
+      <c r="E50">
+        <v>1.1268475090210901</v>
+      </c>
+      <c r="F50">
+        <v>1.1270395632326999</v>
+      </c>
+      <c r="G50">
+        <v>1.1272937821845499</v>
+      </c>
+      <c r="H50">
+        <v>1.1275898379348199</v>
+      </c>
+      <c r="I50">
+        <v>1.12800623230276</v>
+      </c>
+      <c r="J50">
+        <v>1.1286810562601199</v>
+      </c>
+      <c r="K50">
+        <v>1.1295119892296099</v>
+      </c>
+      <c r="L50">
+        <v>1.1305752504769899</v>
+      </c>
+      <c r="M50">
+        <v>1.13198343856123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="B51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D52">
+        <v>0.999</v>
+      </c>
+      <c r="E52">
+        <v>0.99</v>
+      </c>
+      <c r="F52">
+        <v>0.9</v>
+      </c>
+      <c r="G52">
+        <v>0.8</v>
+      </c>
+      <c r="H52">
+        <v>0.7</v>
+      </c>
+      <c r="I52">
+        <v>0.6</v>
+      </c>
+      <c r="J52">
+        <v>0.5</v>
+      </c>
+      <c r="K52">
+        <v>0.4</v>
+      </c>
+      <c r="L52">
+        <v>0.3</v>
+      </c>
+      <c r="M52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" s="11">
+        <v>1.02888139037529</v>
+      </c>
+      <c r="C53" s="11">
+        <v>1.02881824749816</v>
+      </c>
+      <c r="D53" s="11">
+        <v>1.0292493619401499</v>
+      </c>
+      <c r="E53" s="11">
+        <v>1.0306002010907001</v>
+      </c>
+      <c r="F53" s="11">
+        <v>1.0403776264196301</v>
+      </c>
+      <c r="G53" s="11">
+        <v>1.0455536500781699</v>
+      </c>
+      <c r="H53" s="11">
+        <v>1.0502196166931499</v>
+      </c>
+      <c r="I53" s="11">
+        <v>1.05456025548328</v>
+      </c>
+      <c r="J53" s="11">
+        <v>1.0580386809451801</v>
+      </c>
+      <c r="K53" s="11">
+        <v>1.06072869195566</v>
+      </c>
+      <c r="L53" s="11">
+        <v>1.06325182042991</v>
+      </c>
+      <c r="M53" s="11">
+        <v>1.0665343699443</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" s="11">
+        <v>1.0288908441333899</v>
+      </c>
+      <c r="C54" s="11">
+        <v>1.0288602711686301</v>
+      </c>
+      <c r="D54" s="11">
+        <v>1.02880226549612</v>
+      </c>
+      <c r="E54" s="11">
+        <v>1.0302457323054801</v>
+      </c>
+      <c r="F54" s="11">
+        <v>1.0368942578486</v>
+      </c>
+      <c r="G54" s="11">
+        <v>1.0407254732731399</v>
+      </c>
+      <c r="H54" s="11">
+        <v>1.0428459146406599</v>
+      </c>
+      <c r="I54" s="11">
+        <v>1.0440106075208</v>
+      </c>
+      <c r="J54" s="11">
+        <v>1.0446720603447299</v>
+      </c>
+      <c r="K54" s="11">
+        <v>1.0446265725671899</v>
+      </c>
+      <c r="L54" s="11">
+        <v>1.0432536884552599</v>
+      </c>
+      <c r="M54" s="11">
+        <v>1.03960237043072</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55" s="11">
+        <v>1.02896709782511</v>
+      </c>
+      <c r="C55" s="11">
+        <v>1.0289613712810499</v>
+      </c>
+      <c r="D55" s="11">
+        <v>1.0289045845114</v>
+      </c>
+      <c r="E55" s="11">
+        <v>1.02934399304263</v>
+      </c>
+      <c r="F55" s="11">
+        <v>1.0307630197390301</v>
+      </c>
+      <c r="G55" s="11">
+        <v>1.0331979363782999</v>
+      </c>
+      <c r="H55" s="11">
+        <v>1.0354565094261901</v>
+      </c>
+      <c r="I55" s="11">
+        <v>1.0371064775119401</v>
+      </c>
+      <c r="J55" s="11">
+        <v>1.03845198678048</v>
+      </c>
+      <c r="K55" s="11">
+        <v>1.0396339336700899</v>
+      </c>
+      <c r="L55" s="11">
+        <v>1.04062798710354</v>
+      </c>
+      <c r="M55" s="11">
+        <v>1.0413199697934701</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56">
+        <v>100</v>
+      </c>
+      <c r="B56">
+        <v>1.0299088980862201</v>
+      </c>
+      <c r="C56">
+        <v>1.02990835756317</v>
+      </c>
+      <c r="D56">
+        <v>1.02990339428272</v>
+      </c>
+      <c r="E56">
+        <v>1.0298484157397001</v>
+      </c>
+      <c r="F56">
+        <v>1.03034863480575</v>
+      </c>
+      <c r="G56">
+        <v>1.0309928848438601</v>
+      </c>
+      <c r="H56">
+        <v>1.03113240531515</v>
+      </c>
+      <c r="I56">
+        <v>1.0311319416856399</v>
+      </c>
+      <c r="J56">
+        <v>1.0311070133087801</v>
+      </c>
+      <c r="K56">
+        <v>1.0311024084384299</v>
+      </c>
+      <c r="L56">
+        <v>1.0311626762938</v>
+      </c>
+      <c r="M56">
+        <v>1.03133882867862</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57">
+        <v>1000</v>
+      </c>
+      <c r="B57">
+        <v>1.1312136792621199</v>
+      </c>
+      <c r="C57">
+        <v>1.1312142676812</v>
+      </c>
+      <c r="D57">
+        <v>1.1312195669868901</v>
+      </c>
+      <c r="E57">
+        <v>1.1312729141703499</v>
+      </c>
+      <c r="F57">
+        <v>1.13184642295169</v>
+      </c>
+      <c r="G57">
+        <v>1.1325903512022</v>
+      </c>
+      <c r="H57">
+        <v>1.1334764772914701</v>
+      </c>
+      <c r="I57">
+        <v>1.13452007019337</v>
+      </c>
+      <c r="J57">
+        <v>1.1357141560312101</v>
+      </c>
+      <c r="K57">
+        <v>1.13703623230393</v>
+      </c>
+      <c r="L57">
+        <v>1.1384592951241801</v>
+      </c>
+      <c r="M57">
+        <v>1.13995820617467</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="B58" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" s="7">
+        <f>B46-B53</f>
+        <v>-0.87561331080332505</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" ref="C59:M59" si="5">C46-C53</f>
+        <v>-0.84959194409084793</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.55661117169551688</v>
+      </c>
+      <c r="E59" s="7">
+        <f t="shared" si="5"/>
+        <v>9.6763688274049908E-2</v>
+      </c>
+      <c r="F59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.12201379469872986</v>
+      </c>
+      <c r="G59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.13071375975159016</v>
+      </c>
+      <c r="H59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.13939126761574006</v>
+      </c>
+      <c r="I59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.15028568122941999</v>
+      </c>
+      <c r="J59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.16268724131742984</v>
+      </c>
+      <c r="K59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.1854015041986099</v>
+      </c>
+      <c r="L59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.20858560878154009</v>
+      </c>
+      <c r="M59" s="7">
+        <f t="shared" si="5"/>
+        <v>0.21138553731579002</v>
+      </c>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="8"/>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" s="7">
+        <f t="shared" ref="B60:M63" si="6">B47-B54</f>
+        <v>-6.1089584024526911E-2</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" si="6"/>
+        <v>-5.9445760142479154E-2</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="6"/>
+        <v>-3.6505282673005013E-2</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="6"/>
+        <v>8.5772603556429905E-2</v>
+      </c>
+      <c r="F60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11612632354530006</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.12037065717894002</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.12516509221026006</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.13112685377043998</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.13749315386343008</v>
+      </c>
+      <c r="K60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.14460326379494015</v>
+      </c>
+      <c r="L60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.15234641007322014</v>
+      </c>
+      <c r="M60" s="7">
+        <f t="shared" si="6"/>
+        <v>0.15976723458767994</v>
+      </c>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.15167649825175</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.15160053905396009</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.15087787459831992</v>
+      </c>
+      <c r="E61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.13784990444629996</v>
+      </c>
+      <c r="F61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.10749642440099993</v>
+      </c>
+      <c r="G61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11068042969575997</v>
+      </c>
+      <c r="H61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11277736842494002</v>
+      </c>
+      <c r="I61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11369655365551989</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.1134513775980599</v>
+      </c>
+      <c r="K61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11260311539379009</v>
+      </c>
+      <c r="L61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11267994732350006</v>
+      </c>
+      <c r="M61" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11507406218299998</v>
+      </c>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62">
+        <v>100</v>
+      </c>
+      <c r="B62" s="7">
+        <f t="shared" si="6"/>
+        <v>9.4100077941379867E-2</v>
+      </c>
+      <c r="C62" s="7">
+        <f t="shared" si="6"/>
+        <v>9.4102638533690053E-2</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" si="6"/>
+        <v>9.4125595467349887E-2</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" si="6"/>
+        <v>9.4366016643799844E-2</v>
+      </c>
+      <c r="F62" s="7">
+        <f t="shared" si="6"/>
+        <v>9.6836544582939998E-2</v>
+      </c>
+      <c r="G62" s="7">
+        <f t="shared" si="6"/>
+        <v>9.9175985363649799E-2</v>
+      </c>
+      <c r="H62" s="7">
+        <f t="shared" si="6"/>
+        <v>0.10132757330230002</v>
+      </c>
+      <c r="I62" s="7">
+        <f t="shared" si="6"/>
+        <v>0.10311099184299</v>
+      </c>
+      <c r="J62" s="7">
+        <f t="shared" si="6"/>
+        <v>0.10466398310940983</v>
+      </c>
+      <c r="K62" s="7">
+        <f t="shared" si="6"/>
+        <v>0.10628770548114996</v>
+      </c>
+      <c r="L62" s="7">
+        <f t="shared" si="6"/>
+        <v>0.1081664931895201</v>
+      </c>
+      <c r="M62" s="7">
+        <f t="shared" si="6"/>
+        <v>0.11022303600598993</v>
+      </c>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8"/>
+      <c r="R62" s="8"/>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63">
+        <v>1000</v>
+      </c>
+      <c r="B63" s="7">
+        <f t="shared" si="6"/>
+        <v>-4.3853996078098145E-3</v>
+      </c>
+      <c r="C63" s="7">
+        <f t="shared" si="6"/>
+        <v>-4.3857978707200207E-3</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" si="6"/>
+        <v>-4.3893838329200907E-3</v>
+      </c>
+      <c r="E63" s="7">
+        <f t="shared" si="6"/>
+        <v>-4.4254051492598201E-3</v>
+      </c>
+      <c r="F63" s="7">
+        <f t="shared" si="6"/>
+        <v>-4.8068597189900863E-3</v>
+      </c>
+      <c r="G63" s="7">
+        <f t="shared" si="6"/>
+        <v>-5.2965690176500768E-3</v>
+      </c>
+      <c r="H63" s="7">
+        <f t="shared" si="6"/>
+        <v>-5.8866393566501252E-3</v>
+      </c>
+      <c r="I63" s="7">
+        <f t="shared" si="6"/>
+        <v>-6.513837890609997E-3</v>
+      </c>
+      <c r="J63" s="7">
+        <f t="shared" si="6"/>
+        <v>-7.0330997710901233E-3</v>
+      </c>
+      <c r="K63" s="7">
+        <f t="shared" si="6"/>
+        <v>-7.5242430743200917E-3</v>
+      </c>
+      <c r="L63" s="7">
+        <f t="shared" si="6"/>
+        <v>-7.8840446471901693E-3</v>
+      </c>
+      <c r="M63" s="7">
+        <f t="shared" si="6"/>
+        <v>-7.9747676134400702E-3</v>
+      </c>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+    </row>
+    <row r="64" spans="1:18" ht="16" thickBot="1">
+      <c r="A64" s="9"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="9"/>
+    </row>
+    <row r="65" ht="16" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="N38:R42"/>
+    <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B58:M58"/>
+    <mergeCell ref="N59:R63"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="N17:R21"/>
+    <mergeCell ref="B23:M23"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -539,11 +3268,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
@@ -646,7 +3375,7 @@
       <c r="E4">
         <v>7.9396244306663402</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>7.8000740585204804</v>
       </c>
       <c r="G4">
@@ -871,7 +3600,7 @@
       <c r="E10">
         <v>4.58917904262288</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>-0.81669802664189795</v>
       </c>
       <c r="G10">
@@ -1096,7 +3825,7 @@
       <c r="E16">
         <v>0.47263819024463299</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>1.12736388936475</v>
       </c>
       <c r="G16">
@@ -1257,8 +3986,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21">
         <v>1</v>
       </c>
@@ -1361,10 +4090,10 @@
       <c r="E24">
         <v>7.9396244306663402</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>7.8000740585204804</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>7.0531333622822601</v>
       </c>
       <c r="H24">
@@ -1408,7 +4137,7 @@
       <c r="F25">
         <v>7.9393499135033903</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>7.7916514507113099</v>
       </c>
       <c r="H25">
@@ -1586,10 +4315,10 @@
       <c r="E30">
         <v>4.58917904262288</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>-0.81669802664189795</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>-0.81759153017581998</v>
       </c>
       <c r="H30">
@@ -1633,7 +4362,7 @@
       <c r="F31">
         <v>-1.1876981084171401</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>-0.90174379857509601</v>
       </c>
       <c r="H31">
@@ -1811,10 +4540,10 @@
       <c r="E36">
         <v>0.47263819024463299</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>1.12736388936475</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>1.1623914211183599</v>
       </c>
       <c r="H36">
@@ -1858,7 +4587,7 @@
       <c r="F37">
         <v>1.16719389748893</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>1.13825944414003</v>
       </c>
       <c r="H37">
@@ -1972,24 +4701,24 @@
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
@@ -2650,9 +5379,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="F41:J41"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update Fading.xlsx - variances included
</commit_message>
<xml_diff>
--- a/IDA2015/PreliminaryExperiments/Fading.xlsx
+++ b/IDA2015/PreliminaryExperiments/Fading.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-460" windowWidth="32000" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="6560" yWindow="4000" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="VMPvsML" sheetId="2" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="MeanB-Window1" sheetId="3" r:id="rId3"/>
     <sheet name="Beta0-Window1" sheetId="4" r:id="rId4"/>
     <sheet name="Beta1-Window1" sheetId="5" r:id="rId5"/>
+    <sheet name="VarianceB-Window1" sheetId="6" r:id="rId6"/>
+    <sheet name="VarianceA-Window1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="18">
   <si>
     <t xml:space="preserve">WindowSize </t>
   </si>
@@ -71,6 +73,12 @@
   </si>
   <si>
     <t>POSITIVE IS GOOD FOR VMP OVERALL(except at the beginning)</t>
+  </si>
+  <si>
+    <t>Variance of B</t>
+  </si>
+  <si>
+    <t>Variance of A</t>
   </si>
 </sst>
 </file>
@@ -145,7 +153,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -237,8 +245,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -257,8 +273,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -304,6 +321,10 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -349,6 +370,10 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,11 +613,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2129053112"/>
-        <c:axId val="-2128883048"/>
+        <c:axId val="2093123352"/>
+        <c:axId val="2091957496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129053112"/>
+        <c:axId val="2093123352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -602,7 +627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128883048"/>
+        <c:crossAx val="2091957496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -610,7 +635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128883048"/>
+        <c:axId val="2091957496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,7 +646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129053112"/>
+        <c:crossAx val="2093123352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -870,11 +895,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2144423576"/>
-        <c:axId val="2145171160"/>
+        <c:axId val="2093037240"/>
+        <c:axId val="2087477624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2144423576"/>
+        <c:axId val="2093037240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145171160"/>
+        <c:crossAx val="2087477624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -892,7 +917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145171160"/>
+        <c:axId val="2087477624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,7 +928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144423576"/>
+        <c:crossAx val="2093037240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1152,11 +1177,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2143359992"/>
-        <c:axId val="2144377608"/>
+        <c:axId val="2117611864"/>
+        <c:axId val="2093207032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2143359992"/>
+        <c:axId val="2117611864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1166,7 +1191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144377608"/>
+        <c:crossAx val="2093207032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1174,7 +1199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144377608"/>
+        <c:axId val="2093207032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1210,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143359992"/>
+        <c:crossAx val="2117611864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1202,11 +1227,585 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential-VMP</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>VMPvsML!$B$45:$M$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>VMPvsML!$B$67:$M$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.52605225457931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4874725183277</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.31599976243456</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.84386326841068</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.42513237799843</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.66736984124291</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.48348681220078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.12928371046141</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.56011125238829</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.08297383592827</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.771325036714718</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.416701848534184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ML</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>VMPvsML!$B$45:$M$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>VMPvsML!$B$74:$M$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.52235029167482</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4866565107107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.32860207666544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.96298471273172</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.15280809379351</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.62321041794776</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.24520448966573</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.73902089292109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.19433537242763</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.67082142880093</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.19194084972771</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76563007161522</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2141847544"/>
+        <c:axId val="2141850520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2141847544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2141850520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2141850520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2141847544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential-VMP</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>VMPvsML!$B$45:$M$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>VMPvsML!$B$88:$M$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.28859564893407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.88455043739253</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.37310750864604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.213269423062017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.131359962710447</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0752343216226017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0444468902016687</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0253388976695704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.013148544536712</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00567702083137065</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0016466177830416</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>0.000240623660904883</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ML</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>VMPvsML!$B$45:$M$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>VMPvsML!$B$95:$M$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.191102188818641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.190804234144275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.193192791147133</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.217768250857505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.169219037002923</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.132233291214743</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.114496433493671</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0944035799903035</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0705740726256838</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0467090368001592</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0261465327869592</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0110265376967411</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2142664216"/>
+        <c:axId val="2142384952"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2142664216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142384952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2142384952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142664216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="201" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1217,7 +1816,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="201" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1228,7 +1827,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="201" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1239,7 +1838,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9217484" cy="5623145"/>
+    <xdr:ext cx="9214662" cy="5624286"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1266,7 +1865,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9217484" cy="5623145"/>
+    <xdr:ext cx="9214662" cy="5624286"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1293,7 +1892,61 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9217484" cy="5623145"/>
+    <xdr:ext cx="9214662" cy="5624286"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="177800" y="215900"/>
+    <xdr:ext cx="9214662" cy="5624286"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9214662" cy="5624286"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1638,14 +2291,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B53" activeCellId="1" sqref="B46:M46 B53:M53"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4192,9 +4846,1645 @@
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
     </row>
-    <row r="65" ht="16" thickTop="1"/>
+    <row r="65" spans="1:18" ht="16" thickTop="1">
+      <c r="A65" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="4"/>
+    </row>
+    <row r="66" spans="1:18">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D66">
+        <v>0.999</v>
+      </c>
+      <c r="E66">
+        <v>0.99</v>
+      </c>
+      <c r="F66">
+        <v>0.9</v>
+      </c>
+      <c r="G66">
+        <v>0.8</v>
+      </c>
+      <c r="H66">
+        <v>0.7</v>
+      </c>
+      <c r="I66">
+        <v>0.6</v>
+      </c>
+      <c r="J66">
+        <v>0.5</v>
+      </c>
+      <c r="K66">
+        <v>0.4</v>
+      </c>
+      <c r="L66">
+        <v>0.3</v>
+      </c>
+      <c r="M66">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>6.5260522545793096</v>
+      </c>
+      <c r="C67">
+        <v>6.4874725183277002</v>
+      </c>
+      <c r="D67">
+        <v>6.3159997624345596</v>
+      </c>
+      <c r="E67">
+        <v>5.8438632684106802</v>
+      </c>
+      <c r="F67">
+        <v>3.42513237799843</v>
+      </c>
+      <c r="G67">
+        <v>2.6673698412429099</v>
+      </c>
+      <c r="H67">
+        <v>2.48348681220078</v>
+      </c>
+      <c r="I67">
+        <v>2.1292837104614102</v>
+      </c>
+      <c r="J67">
+        <v>1.5601112523882901</v>
+      </c>
+      <c r="K67">
+        <v>1.0829738359282699</v>
+      </c>
+      <c r="L67">
+        <v>0.77132503671471797</v>
+      </c>
+      <c r="M67">
+        <v>0.41670184853418402</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>6.5253608660533304</v>
+      </c>
+      <c r="C68">
+        <v>6.5062683153696499</v>
+      </c>
+      <c r="D68">
+        <v>6.3672914078282101</v>
+      </c>
+      <c r="E68">
+        <v>6.14354670631801</v>
+      </c>
+      <c r="F68">
+        <v>4.3847986342107896</v>
+      </c>
+      <c r="G68">
+        <v>3.1772799923456501</v>
+      </c>
+      <c r="H68">
+        <v>2.6173087244463402</v>
+      </c>
+      <c r="I68">
+        <v>2.3987905735114898</v>
+      </c>
+      <c r="J68">
+        <v>2.2669477982042898</v>
+      </c>
+      <c r="K68">
+        <v>1.86445526589504</v>
+      </c>
+      <c r="L68">
+        <v>1.0647619445484799</v>
+      </c>
+      <c r="M68">
+        <v>0.44361356286175602</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>6.52231115468319</v>
+      </c>
+      <c r="C69">
+        <v>6.51868365883902</v>
+      </c>
+      <c r="D69">
+        <v>6.4853689137341002</v>
+      </c>
+      <c r="E69">
+        <v>6.3165087303040801</v>
+      </c>
+      <c r="F69">
+        <v>5.7988583671996903</v>
+      </c>
+      <c r="G69">
+        <v>5.2930380871086502</v>
+      </c>
+      <c r="H69">
+        <v>4.8553946198551401</v>
+      </c>
+      <c r="I69">
+        <v>4.3949370650539903</v>
+      </c>
+      <c r="J69">
+        <v>3.9020637589167699</v>
+      </c>
+      <c r="K69">
+        <v>3.38248293847986</v>
+      </c>
+      <c r="L69">
+        <v>2.8249972230834102</v>
+      </c>
+      <c r="M69">
+        <v>2.1805209661366098</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="A70">
+        <v>100</v>
+      </c>
+      <c r="B70">
+        <v>6.5212997408677396</v>
+      </c>
+      <c r="C70">
+        <v>6.5209401723233702</v>
+      </c>
+      <c r="D70">
+        <v>6.5176890789453497</v>
+      </c>
+      <c r="E70">
+        <v>6.4842777269898102</v>
+      </c>
+      <c r="F70">
+        <v>6.3073099901538701</v>
+      </c>
+      <c r="G70">
+        <v>6.2690347372523796</v>
+      </c>
+      <c r="H70">
+        <v>6.2038383928794598</v>
+      </c>
+      <c r="I70">
+        <v>6.1022196978033003</v>
+      </c>
+      <c r="J70">
+        <v>5.9689124363629702</v>
+      </c>
+      <c r="K70">
+        <v>5.8049789343472096</v>
+      </c>
+      <c r="L70">
+        <v>5.60165247944395</v>
+      </c>
+      <c r="M70">
+        <v>5.3199509117522696</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
+      <c r="A71">
+        <v>1000</v>
+      </c>
+      <c r="B71">
+        <v>6.5218152555798499</v>
+      </c>
+      <c r="C71">
+        <v>6.5217805400189004</v>
+      </c>
+      <c r="D71">
+        <v>6.5214677430014296</v>
+      </c>
+      <c r="E71">
+        <v>6.5183046179043096</v>
+      </c>
+      <c r="F71">
+        <v>6.4834453661742302</v>
+      </c>
+      <c r="G71">
+        <v>6.4398900348077701</v>
+      </c>
+      <c r="H71">
+        <v>6.3957526047927002</v>
+      </c>
+      <c r="I71">
+        <v>6.3556840778658099</v>
+      </c>
+      <c r="J71">
+        <v>6.3222801801891899</v>
+      </c>
+      <c r="K71">
+        <v>6.2954415458749304</v>
+      </c>
+      <c r="L71">
+        <v>6.2724894082792497</v>
+      </c>
+      <c r="M71">
+        <v>6.2461103620244796</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="B72" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+    </row>
+    <row r="73" spans="1:18">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D73">
+        <v>0.999</v>
+      </c>
+      <c r="E73">
+        <v>0.99</v>
+      </c>
+      <c r="F73">
+        <v>0.9</v>
+      </c>
+      <c r="G73">
+        <v>0.8</v>
+      </c>
+      <c r="H73">
+        <v>0.7</v>
+      </c>
+      <c r="I73">
+        <v>0.6</v>
+      </c>
+      <c r="J73">
+        <v>0.5</v>
+      </c>
+      <c r="K73">
+        <v>0.4</v>
+      </c>
+      <c r="L73">
+        <v>0.3</v>
+      </c>
+      <c r="M73">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>6.5223502916748197</v>
+      </c>
+      <c r="C74">
+        <v>6.4866565107107004</v>
+      </c>
+      <c r="D74">
+        <v>6.3286020766654403</v>
+      </c>
+      <c r="E74">
+        <v>5.9629847127317204</v>
+      </c>
+      <c r="F74">
+        <v>4.1528080937935101</v>
+      </c>
+      <c r="G74">
+        <v>3.6232104179477602</v>
+      </c>
+      <c r="H74">
+        <v>3.2452044896657299</v>
+      </c>
+      <c r="I74">
+        <v>2.73902089292109</v>
+      </c>
+      <c r="J74">
+        <v>2.1943353724276302</v>
+      </c>
+      <c r="K74">
+        <v>1.67082142880093</v>
+      </c>
+      <c r="L74">
+        <v>1.19194084972771</v>
+      </c>
+      <c r="M74">
+        <v>0.76563007161522001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75">
+        <v>6.5223502916746803</v>
+      </c>
+      <c r="C75">
+        <v>6.5046298387404198</v>
+      </c>
+      <c r="D75">
+        <v>6.3735814988025501</v>
+      </c>
+      <c r="E75">
+        <v>6.2057314505679297</v>
+      </c>
+      <c r="F75">
+        <v>4.95426418169572</v>
+      </c>
+      <c r="G75">
+        <v>4.2026519828523501</v>
+      </c>
+      <c r="H75">
+        <v>3.9285629000468898</v>
+      </c>
+      <c r="I75">
+        <v>3.7792244328256199</v>
+      </c>
+      <c r="J75">
+        <v>3.5609495399000002</v>
+      </c>
+      <c r="K75">
+        <v>3.2294387181822199</v>
+      </c>
+      <c r="L75">
+        <v>2.8029672951815998</v>
+      </c>
+      <c r="M75">
+        <v>2.30230461698741</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
+      <c r="A76">
+        <v>10</v>
+      </c>
+      <c r="B76">
+        <v>6.5223502916749903</v>
+      </c>
+      <c r="C76">
+        <v>6.5188520456455796</v>
+      </c>
+      <c r="D76">
+        <v>6.48669083255926</v>
+      </c>
+      <c r="E76">
+        <v>6.3289197301226903</v>
+      </c>
+      <c r="F76">
+        <v>5.9269587474560899</v>
+      </c>
+      <c r="G76">
+        <v>5.5440478157524797</v>
+      </c>
+      <c r="H76">
+        <v>5.2245552455912403</v>
+      </c>
+      <c r="I76">
+        <v>4.8885378155846499</v>
+      </c>
+      <c r="J76">
+        <v>4.5402741932719204</v>
+      </c>
+      <c r="K76">
+        <v>4.2034532202169297</v>
+      </c>
+      <c r="L76">
+        <v>3.9009584315307402</v>
+      </c>
+      <c r="M76">
+        <v>3.6457030133031201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
+      <c r="A77">
+        <v>100</v>
+      </c>
+      <c r="B77">
+        <v>6.5223502916747904</v>
+      </c>
+      <c r="C77">
+        <v>6.52199915053769</v>
+      </c>
+      <c r="D77">
+        <v>6.5188255388182199</v>
+      </c>
+      <c r="E77">
+        <v>6.48624752651902</v>
+      </c>
+      <c r="F77">
+        <v>6.3214734661833303</v>
+      </c>
+      <c r="G77">
+        <v>6.2993444434155696</v>
+      </c>
+      <c r="H77">
+        <v>6.2552659620461597</v>
+      </c>
+      <c r="I77">
+        <v>6.1820313378566398</v>
+      </c>
+      <c r="J77">
+        <v>6.0866264868572397</v>
+      </c>
+      <c r="K77">
+        <v>5.9751555633165898</v>
+      </c>
+      <c r="L77">
+        <v>5.8528459436019604</v>
+      </c>
+      <c r="M77">
+        <v>5.7243241392380799</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
+      <c r="A78">
+        <v>1000</v>
+      </c>
+      <c r="B78">
+        <v>6.52235029167481</v>
+      </c>
+      <c r="C78">
+        <v>6.5223167349484701</v>
+      </c>
+      <c r="D78">
+        <v>6.5220143798972403</v>
+      </c>
+      <c r="E78">
+        <v>6.5189569182084002</v>
+      </c>
+      <c r="F78">
+        <v>6.4852884035368401</v>
+      </c>
+      <c r="G78">
+        <v>6.4433720838125703</v>
+      </c>
+      <c r="H78">
+        <v>6.40124241785196</v>
+      </c>
+      <c r="I78">
+        <v>6.36367938018273</v>
+      </c>
+      <c r="J78">
+        <v>6.3337005984116903</v>
+      </c>
+      <c r="K78">
+        <v>6.3121728232429204</v>
+      </c>
+      <c r="L78">
+        <v>6.2985870042797396</v>
+      </c>
+      <c r="M78">
+        <v>6.2918649074527204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
+      <c r="B79" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="11"/>
+      <c r="L79" s="11"/>
+      <c r="M79" s="11"/>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80" s="5">
+        <f>B67-B74</f>
+        <v>3.701962904489875E-3</v>
+      </c>
+      <c r="C80" s="5">
+        <f t="shared" ref="C80:M80" si="9">C67-C74</f>
+        <v>8.1600761699984758E-4</v>
+      </c>
+      <c r="D80" s="5">
+        <f t="shared" si="9"/>
+        <v>-1.2602314230880651E-2</v>
+      </c>
+      <c r="E80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.11912144432104022</v>
+      </c>
+      <c r="F80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.72767571579508017</v>
+      </c>
+      <c r="G80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.95584057670485034</v>
+      </c>
+      <c r="H80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.76171767746494989</v>
+      </c>
+      <c r="I80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.60973718245967978</v>
+      </c>
+      <c r="J80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.63422412003934014</v>
+      </c>
+      <c r="K80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.58784759287266009</v>
+      </c>
+      <c r="L80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.420615813012992</v>
+      </c>
+      <c r="M80" s="5">
+        <f t="shared" si="9"/>
+        <v>-0.34892822308103599</v>
+      </c>
+      <c r="N80" s="9"/>
+      <c r="O80" s="9"/>
+      <c r="P80" s="9"/>
+      <c r="Q80" s="9"/>
+      <c r="R80" s="9"/>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81" s="5">
+        <f>B68-B75</f>
+        <v>3.0105743786501549E-3</v>
+      </c>
+      <c r="C81" s="5">
+        <f t="shared" ref="C81:M81" si="10">C68-C75</f>
+        <v>1.6384766292301123E-3</v>
+      </c>
+      <c r="D81" s="5">
+        <f t="shared" si="10"/>
+        <v>-6.290090974339968E-3</v>
+      </c>
+      <c r="E81" s="5">
+        <f t="shared" si="10"/>
+        <v>-6.218474424991971E-2</v>
+      </c>
+      <c r="F81" s="5">
+        <f t="shared" si="10"/>
+        <v>-0.56946554748493039</v>
+      </c>
+      <c r="G81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.0253719905067</v>
+      </c>
+      <c r="H81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.3112541756005496</v>
+      </c>
+      <c r="I81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.3804338593141301</v>
+      </c>
+      <c r="J81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.2940017416957104</v>
+      </c>
+      <c r="K81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.36498345228718</v>
+      </c>
+      <c r="L81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.7382053506331199</v>
+      </c>
+      <c r="M81" s="5">
+        <f t="shared" si="10"/>
+        <v>-1.8586910541256541</v>
+      </c>
+      <c r="N81" s="9"/>
+      <c r="O81" s="9"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="9"/>
+      <c r="R81" s="9"/>
+    </row>
+    <row r="82" spans="1:18">
+      <c r="A82">
+        <v>10</v>
+      </c>
+      <c r="B82" s="5">
+        <f>B69-B76</f>
+        <v>-3.9136991800248211E-5</v>
+      </c>
+      <c r="C82" s="5">
+        <f t="shared" ref="C82:M82" si="11">C69-C76</f>
+        <v>-1.6838680655961724E-4</v>
+      </c>
+      <c r="D82" s="5">
+        <f t="shared" si="11"/>
+        <v>-1.3219188251598624E-3</v>
+      </c>
+      <c r="E82" s="5">
+        <f t="shared" si="11"/>
+        <v>-1.2410999818610158E-2</v>
+      </c>
+      <c r="F82" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.12810038025639958</v>
+      </c>
+      <c r="G82" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.25100972864382953</v>
+      </c>
+      <c r="H82" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.3691606257361002</v>
+      </c>
+      <c r="I82" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.49360075053065966</v>
+      </c>
+      <c r="J82" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.63821043435515046</v>
+      </c>
+      <c r="K82" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.82097028173706965</v>
+      </c>
+      <c r="L82" s="5">
+        <f t="shared" si="11"/>
+        <v>-1.07596120844733</v>
+      </c>
+      <c r="M82" s="5">
+        <f t="shared" si="11"/>
+        <v>-1.4651820471665102</v>
+      </c>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9"/>
+      <c r="R82" s="9"/>
+    </row>
+    <row r="83" spans="1:18">
+      <c r="A83">
+        <v>100</v>
+      </c>
+      <c r="B83" s="5">
+        <f>B70-B77</f>
+        <v>-1.050550807050854E-3</v>
+      </c>
+      <c r="C83" s="5">
+        <f t="shared" ref="C83:M83" si="12">C70-C77</f>
+        <v>-1.0589782143197723E-3</v>
+      </c>
+      <c r="D83" s="5">
+        <f t="shared" si="12"/>
+        <v>-1.1364598728702546E-3</v>
+      </c>
+      <c r="E83" s="5">
+        <f t="shared" si="12"/>
+        <v>-1.9697995292098369E-3</v>
+      </c>
+      <c r="F83" s="5">
+        <f t="shared" si="12"/>
+        <v>-1.416347602946022E-2</v>
+      </c>
+      <c r="G83" s="5">
+        <f t="shared" si="12"/>
+        <v>-3.0309706163190064E-2</v>
+      </c>
+      <c r="H83" s="5">
+        <f t="shared" si="12"/>
+        <v>-5.1427569166699882E-2</v>
+      </c>
+      <c r="I83" s="5">
+        <f t="shared" si="12"/>
+        <v>-7.9811640053339516E-2</v>
+      </c>
+      <c r="J83" s="5">
+        <f t="shared" si="12"/>
+        <v>-0.11771405049426953</v>
+      </c>
+      <c r="K83" s="5">
+        <f t="shared" si="12"/>
+        <v>-0.17017662896938024</v>
+      </c>
+      <c r="L83" s="5">
+        <f t="shared" si="12"/>
+        <v>-0.25119346415801047</v>
+      </c>
+      <c r="M83" s="5">
+        <f t="shared" si="12"/>
+        <v>-0.40437322748581028</v>
+      </c>
+      <c r="N83" s="9"/>
+      <c r="O83" s="9"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="9"/>
+      <c r="R83" s="9"/>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84">
+        <v>1000</v>
+      </c>
+      <c r="B84" s="5">
+        <f t="shared" ref="B84:M84" si="13">B71-B78</f>
+        <v>-5.3503609496008409E-4</v>
+      </c>
+      <c r="C84" s="5">
+        <f t="shared" si="13"/>
+        <v>-5.3619492956968884E-4</v>
+      </c>
+      <c r="D84" s="5">
+        <f t="shared" si="13"/>
+        <v>-5.4663689581069264E-4</v>
+      </c>
+      <c r="E84" s="5">
+        <f t="shared" si="13"/>
+        <v>-6.523003040905806E-4</v>
+      </c>
+      <c r="F84" s="5">
+        <f t="shared" si="13"/>
+        <v>-1.8430373626099339E-3</v>
+      </c>
+      <c r="G84" s="5">
+        <f t="shared" si="13"/>
+        <v>-3.4820490048002029E-3</v>
+      </c>
+      <c r="H84" s="5">
+        <f t="shared" si="13"/>
+        <v>-5.4898130592597738E-3</v>
+      </c>
+      <c r="I84" s="5">
+        <f t="shared" si="13"/>
+        <v>-7.9953023169201387E-3</v>
+      </c>
+      <c r="J84" s="5">
+        <f t="shared" si="13"/>
+        <v>-1.1420418222500395E-2</v>
+      </c>
+      <c r="K84" s="5">
+        <f t="shared" si="13"/>
+        <v>-1.6731277367989961E-2</v>
+      </c>
+      <c r="L84" s="5">
+        <f t="shared" si="13"/>
+        <v>-2.6097596000489887E-2</v>
+      </c>
+      <c r="M84" s="5">
+        <f t="shared" si="13"/>
+        <v>-4.5754545428240867E-2</v>
+      </c>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9"/>
+      <c r="P84" s="9"/>
+      <c r="Q84" s="9"/>
+      <c r="R84" s="9"/>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="11"/>
+      <c r="K86" s="11"/>
+      <c r="L86" s="11"/>
+      <c r="M86" s="11"/>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D87">
+        <v>0.999</v>
+      </c>
+      <c r="E87">
+        <v>0.99</v>
+      </c>
+      <c r="F87">
+        <v>0.9</v>
+      </c>
+      <c r="G87">
+        <v>0.8</v>
+      </c>
+      <c r="H87">
+        <v>0.7</v>
+      </c>
+      <c r="I87">
+        <v>0.6</v>
+      </c>
+      <c r="J87">
+        <v>0.5</v>
+      </c>
+      <c r="K87">
+        <v>0.4</v>
+      </c>
+      <c r="L87">
+        <v>0.3</v>
+      </c>
+      <c r="M87">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>7.28859564893407</v>
+      </c>
+      <c r="C88">
+        <v>6.8845504373925301</v>
+      </c>
+      <c r="D88">
+        <v>3.37310750864604</v>
+      </c>
+      <c r="E88">
+        <v>0.21326942306201699</v>
+      </c>
+      <c r="F88">
+        <v>0.131359962710447</v>
+      </c>
+      <c r="G88">
+        <v>7.5234321622601699E-2</v>
+      </c>
+      <c r="H88">
+        <v>4.4446890201668698E-2</v>
+      </c>
+      <c r="I88">
+        <v>2.5338897669570402E-2</v>
+      </c>
+      <c r="J88">
+        <v>1.3148544536711999E-2</v>
+      </c>
+      <c r="K88">
+        <v>5.6770208313706499E-3</v>
+      </c>
+      <c r="L88">
+        <v>1.6466177830416001E-3</v>
+      </c>
+      <c r="M88" s="12">
+        <v>2.4062366090488299E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="B89">
+        <v>0.39191478148946401</v>
+      </c>
+      <c r="C89">
+        <v>0.38669101926577198</v>
+      </c>
+      <c r="D89">
+        <v>0.33763688564444899</v>
+      </c>
+      <c r="E89">
+        <v>0.206011954263496</v>
+      </c>
+      <c r="F89">
+        <v>0.185097478969767</v>
+      </c>
+      <c r="G89">
+        <v>0.13863959391849001</v>
+      </c>
+      <c r="H89">
+        <v>0.106727602511702</v>
+      </c>
+      <c r="I89">
+        <v>8.2777261702301694E-2</v>
+      </c>
+      <c r="J89">
+        <v>6.3605837326623393E-2</v>
+      </c>
+      <c r="K89">
+        <v>4.7603484422679102E-2</v>
+      </c>
+      <c r="L89">
+        <v>3.3777026526103399E-2</v>
+      </c>
+      <c r="M89">
+        <v>2.1671413814649099E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="A90">
+        <v>10</v>
+      </c>
+      <c r="B90">
+        <v>0.20987202725009199</v>
+      </c>
+      <c r="C90">
+        <v>0.20967424815416699</v>
+      </c>
+      <c r="D90">
+        <v>0.20801647561582301</v>
+      </c>
+      <c r="E90">
+        <v>0.19892789796402199</v>
+      </c>
+      <c r="F90">
+        <v>0.21277446251191701</v>
+      </c>
+      <c r="G90">
+        <v>0.21374504527381299</v>
+      </c>
+      <c r="H90">
+        <v>0.19915567045970201</v>
+      </c>
+      <c r="I90">
+        <v>0.18000396239303801</v>
+      </c>
+      <c r="J90">
+        <v>0.159310718631715</v>
+      </c>
+      <c r="K90">
+        <v>0.13730667795170501</v>
+      </c>
+      <c r="L90">
+        <v>0.113346343442829</v>
+      </c>
+      <c r="M90">
+        <v>8.6244805793118107E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
+      <c r="A91">
+        <v>100</v>
+      </c>
+      <c r="B91">
+        <v>0.19168442037865499</v>
+      </c>
+      <c r="C91">
+        <v>0.191678904123296</v>
+      </c>
+      <c r="D91">
+        <v>0.19163215471005399</v>
+      </c>
+      <c r="E91">
+        <v>0.19130479368446601</v>
+      </c>
+      <c r="F91">
+        <v>0.19363871333156499</v>
+      </c>
+      <c r="G91">
+        <v>0.19636010823150399</v>
+      </c>
+      <c r="H91">
+        <v>0.199709487290259</v>
+      </c>
+      <c r="I91">
+        <v>0.204312003011002</v>
+      </c>
+      <c r="J91">
+        <v>0.20993438164581801</v>
+      </c>
+      <c r="K91">
+        <v>0.21593532286383299</v>
+      </c>
+      <c r="L91">
+        <v>0.22124644618519701</v>
+      </c>
+      <c r="M91">
+        <v>0.22347621397980799</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
+      <c r="A92">
+        <v>1000</v>
+      </c>
+      <c r="B92">
+        <v>0.19145604931566099</v>
+      </c>
+      <c r="C92">
+        <v>0.19145553056970499</v>
+      </c>
+      <c r="D92">
+        <v>0.191450869744449</v>
+      </c>
+      <c r="E92">
+        <v>0.19140505626541601</v>
+      </c>
+      <c r="F92">
+        <v>0.19103932982083799</v>
+      </c>
+      <c r="G92">
+        <v>0.19086853241371901</v>
+      </c>
+      <c r="H92">
+        <v>0.19095650848137</v>
+      </c>
+      <c r="I92">
+        <v>0.191254236890922</v>
+      </c>
+      <c r="J92">
+        <v>0.19168356199247299</v>
+      </c>
+      <c r="K92">
+        <v>0.192194333231858</v>
+      </c>
+      <c r="L92">
+        <v>0.192735398887592</v>
+      </c>
+      <c r="M92">
+        <v>0.19314804778648501</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
+      <c r="B93" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="11"/>
+      <c r="L93" s="11"/>
+      <c r="M93" s="11"/>
+    </row>
+    <row r="94" spans="1:18">
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D94">
+        <v>0.999</v>
+      </c>
+      <c r="E94">
+        <v>0.99</v>
+      </c>
+      <c r="F94">
+        <v>0.9</v>
+      </c>
+      <c r="G94">
+        <v>0.8</v>
+      </c>
+      <c r="H94">
+        <v>0.7</v>
+      </c>
+      <c r="I94">
+        <v>0.6</v>
+      </c>
+      <c r="J94">
+        <v>0.5</v>
+      </c>
+      <c r="K94">
+        <v>0.4</v>
+      </c>
+      <c r="L94">
+        <v>0.3</v>
+      </c>
+      <c r="M94">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>0.19110218881864099</v>
+      </c>
+      <c r="C95">
+        <v>0.190804234144275</v>
+      </c>
+      <c r="D95">
+        <v>0.193192791147133</v>
+      </c>
+      <c r="E95">
+        <v>0.21776825085750501</v>
+      </c>
+      <c r="F95">
+        <v>0.16921903700292301</v>
+      </c>
+      <c r="G95">
+        <v>0.132233291214743</v>
+      </c>
+      <c r="H95">
+        <v>0.114496433493671</v>
+      </c>
+      <c r="I95">
+        <v>9.4403579990303493E-2</v>
+      </c>
+      <c r="J95">
+        <v>7.0574072625683798E-2</v>
+      </c>
+      <c r="K95">
+        <v>4.6709036800159198E-2</v>
+      </c>
+      <c r="L95">
+        <v>2.6146532786959199E-2</v>
+      </c>
+      <c r="M95">
+        <v>1.10265376967411E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>0.191102188818813</v>
+      </c>
+      <c r="C96">
+        <v>0.19091700913808399</v>
+      </c>
+      <c r="D96">
+        <v>0.191606212304618</v>
+      </c>
+      <c r="E96">
+        <v>0.204310226841357</v>
+      </c>
+      <c r="F96">
+        <v>0.20506514759677399</v>
+      </c>
+      <c r="G96">
+        <v>0.165800566195661</v>
+      </c>
+      <c r="H96">
+        <v>0.139198848188717</v>
+      </c>
+      <c r="I96">
+        <v>0.123252481220196</v>
+      </c>
+      <c r="J96">
+        <v>0.110588110046172</v>
+      </c>
+      <c r="K96">
+        <v>9.6262363909640394E-2</v>
+      </c>
+      <c r="L96">
+        <v>7.8404673780397602E-2</v>
+      </c>
+      <c r="M96">
+        <v>5.7354642629659398E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97">
+        <v>10</v>
+      </c>
+      <c r="B97">
+        <v>0.19110218881883501</v>
+      </c>
+      <c r="C97">
+        <v>0.19105936382313901</v>
+      </c>
+      <c r="D97">
+        <v>0.190803377568212</v>
+      </c>
+      <c r="E97">
+        <v>0.193166397031449</v>
+      </c>
+      <c r="F97">
+        <v>0.21841134751644301</v>
+      </c>
+      <c r="G97">
+        <v>0.2251046427667</v>
+      </c>
+      <c r="H97">
+        <v>0.21541655133714299</v>
+      </c>
+      <c r="I97">
+        <v>0.20082276595103099</v>
+      </c>
+      <c r="J97">
+        <v>0.18414038599167201</v>
+      </c>
+      <c r="K97">
+        <v>0.165952745228056</v>
+      </c>
+      <c r="L97">
+        <v>0.14700670748122499</v>
+      </c>
+      <c r="M97">
+        <v>0.128483583871289</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98">
+        <v>100</v>
+      </c>
+      <c r="B98">
+        <v>0.1911021888186</v>
+      </c>
+      <c r="C98">
+        <v>0.19109773424975501</v>
+      </c>
+      <c r="D98">
+        <v>0.19105891240841999</v>
+      </c>
+      <c r="E98">
+        <v>0.19079957764930899</v>
+      </c>
+      <c r="F98">
+        <v>0.193278267089388</v>
+      </c>
+      <c r="G98">
+        <v>0.19638639686311299</v>
+      </c>
+      <c r="H98">
+        <v>0.200532857098288</v>
+      </c>
+      <c r="I98">
+        <v>0.206174020575353</v>
+      </c>
+      <c r="J98">
+        <v>0.21318774152266901</v>
+      </c>
+      <c r="K98">
+        <v>0.22124467229499201</v>
+      </c>
+      <c r="L98">
+        <v>0.229993241875177</v>
+      </c>
+      <c r="M98">
+        <v>0.23908199647512601</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99">
+        <v>1000</v>
+      </c>
+      <c r="B99">
+        <v>0.19110218881865901</v>
+      </c>
+      <c r="C99">
+        <v>0.19110174676879399</v>
+      </c>
+      <c r="D99">
+        <v>0.19109777596688399</v>
+      </c>
+      <c r="E99">
+        <v>0.191058838190382</v>
+      </c>
+      <c r="F99">
+        <v>0.19075866209254599</v>
+      </c>
+      <c r="G99">
+        <v>0.190652290486577</v>
+      </c>
+      <c r="H99">
+        <v>0.19079572842324799</v>
+      </c>
+      <c r="I99">
+        <v>0.19114573785133601</v>
+      </c>
+      <c r="J99">
+        <v>0.191648261156665</v>
+      </c>
+      <c r="K99">
+        <v>0.192283205002789</v>
+      </c>
+      <c r="L99">
+        <v>0.193074375105727</v>
+      </c>
+      <c r="M99">
+        <v>0.194071854526598</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="B100" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="11"/>
+      <c r="K100" s="11"/>
+      <c r="L100" s="11"/>
+      <c r="M100" s="11"/>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101" s="5">
+        <f>B88-B95</f>
+        <v>7.0974934601154294</v>
+      </c>
+      <c r="C101" s="5">
+        <f t="shared" ref="C101:M101" si="14">C88-C95</f>
+        <v>6.6937462032482555</v>
+      </c>
+      <c r="D101" s="5">
+        <f t="shared" si="14"/>
+        <v>3.1799147174989071</v>
+      </c>
+      <c r="E101" s="5">
+        <f t="shared" si="14"/>
+        <v>-4.4988277954880196E-3</v>
+      </c>
+      <c r="F101" s="5">
+        <f t="shared" si="14"/>
+        <v>-3.7859074292476008E-2</v>
+      </c>
+      <c r="G101" s="5">
+        <f t="shared" si="14"/>
+        <v>-5.6998969592141305E-2</v>
+      </c>
+      <c r="H101" s="5">
+        <f t="shared" si="14"/>
+        <v>-7.0049543292002303E-2</v>
+      </c>
+      <c r="I101" s="5">
+        <f t="shared" si="14"/>
+        <v>-6.9064682320733095E-2</v>
+      </c>
+      <c r="J101" s="5">
+        <f t="shared" si="14"/>
+        <v>-5.7425528088971799E-2</v>
+      </c>
+      <c r="K101" s="5">
+        <f t="shared" si="14"/>
+        <v>-4.1032015968788547E-2</v>
+      </c>
+      <c r="L101" s="5">
+        <f t="shared" si="14"/>
+        <v>-2.4499915003917599E-2</v>
+      </c>
+      <c r="M101" s="5">
+        <f t="shared" si="14"/>
+        <v>-1.0785914035836217E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102" s="5">
+        <f>B89-B96</f>
+        <v>0.20081259267065102</v>
+      </c>
+      <c r="C102" s="5">
+        <f t="shared" ref="C102:M102" si="15">C89-C96</f>
+        <v>0.195774010127688</v>
+      </c>
+      <c r="D102" s="5">
+        <f t="shared" si="15"/>
+        <v>0.146030673339831</v>
+      </c>
+      <c r="E102" s="5">
+        <f t="shared" si="15"/>
+        <v>1.7017274221390044E-3</v>
+      </c>
+      <c r="F102" s="5">
+        <f t="shared" si="15"/>
+        <v>-1.9967668627006996E-2</v>
+      </c>
+      <c r="G102" s="5">
+        <f t="shared" si="15"/>
+        <v>-2.7160972277170986E-2</v>
+      </c>
+      <c r="H102" s="5">
+        <f t="shared" si="15"/>
+        <v>-3.2471245677014995E-2</v>
+      </c>
+      <c r="I102" s="5">
+        <f t="shared" si="15"/>
+        <v>-4.0475219517894304E-2</v>
+      </c>
+      <c r="J102" s="5">
+        <f t="shared" si="15"/>
+        <v>-4.6982272719548607E-2</v>
+      </c>
+      <c r="K102" s="5">
+        <f t="shared" si="15"/>
+        <v>-4.8658879486961293E-2</v>
+      </c>
+      <c r="L102" s="5">
+        <f t="shared" si="15"/>
+        <v>-4.4627647254294203E-2</v>
+      </c>
+      <c r="M102" s="5">
+        <f t="shared" si="15"/>
+        <v>-3.56832288150103E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103">
+        <v>10</v>
+      </c>
+      <c r="B103" s="5">
+        <f>B90-B97</f>
+        <v>1.8769838431256985E-2</v>
+      </c>
+      <c r="C103" s="5">
+        <f t="shared" ref="C103:M103" si="16">C90-C97</f>
+        <v>1.8614884331027981E-2</v>
+      </c>
+      <c r="D103" s="5">
+        <f t="shared" si="16"/>
+        <v>1.7213098047611008E-2</v>
+      </c>
+      <c r="E103" s="5">
+        <f t="shared" si="16"/>
+        <v>5.7615009325729938E-3</v>
+      </c>
+      <c r="F103" s="5">
+        <f t="shared" si="16"/>
+        <v>-5.6368850045259988E-3</v>
+      </c>
+      <c r="G103" s="5">
+        <f t="shared" si="16"/>
+        <v>-1.1359597492887008E-2</v>
+      </c>
+      <c r="H103" s="5">
+        <f t="shared" si="16"/>
+        <v>-1.6260880877440986E-2</v>
+      </c>
+      <c r="I103" s="5">
+        <f t="shared" si="16"/>
+        <v>-2.0818803557992982E-2</v>
+      </c>
+      <c r="J103" s="5">
+        <f t="shared" si="16"/>
+        <v>-2.4829667359957008E-2</v>
+      </c>
+      <c r="K103" s="5">
+        <f t="shared" si="16"/>
+        <v>-2.8646067276350995E-2</v>
+      </c>
+      <c r="L103" s="5">
+        <f t="shared" si="16"/>
+        <v>-3.3660364038395993E-2</v>
+      </c>
+      <c r="M103" s="5">
+        <f t="shared" si="16"/>
+        <v>-4.2238778078170891E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104">
+        <v>100</v>
+      </c>
+      <c r="B104" s="5">
+        <f>B91-B98</f>
+        <v>5.8223156005499099E-4</v>
+      </c>
+      <c r="C104" s="5">
+        <f t="shared" ref="C104:M104" si="17">C91-C98</f>
+        <v>5.8116987354098204E-4</v>
+      </c>
+      <c r="D104" s="5">
+        <f t="shared" si="17"/>
+        <v>5.7324230163399714E-4</v>
+      </c>
+      <c r="E104" s="5">
+        <f t="shared" si="17"/>
+        <v>5.0521603515701896E-4</v>
+      </c>
+      <c r="F104" s="5">
+        <f t="shared" si="17"/>
+        <v>3.6044624217698717E-4</v>
+      </c>
+      <c r="G104" s="5">
+        <f t="shared" si="17"/>
+        <v>-2.6288631609000523E-5</v>
+      </c>
+      <c r="H104" s="5">
+        <f t="shared" si="17"/>
+        <v>-8.2336980802899529E-4</v>
+      </c>
+      <c r="I104" s="5">
+        <f t="shared" si="17"/>
+        <v>-1.862017564351004E-3</v>
+      </c>
+      <c r="J104" s="5">
+        <f t="shared" si="17"/>
+        <v>-3.2533598768509919E-3</v>
+      </c>
+      <c r="K104" s="5">
+        <f t="shared" si="17"/>
+        <v>-5.3093494311590161E-3</v>
+      </c>
+      <c r="L104" s="5">
+        <f t="shared" si="17"/>
+        <v>-8.7467956899799915E-3</v>
+      </c>
+      <c r="M104" s="5">
+        <f t="shared" si="17"/>
+        <v>-1.5605782495318021E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105">
+        <v>1000</v>
+      </c>
+      <c r="B105" s="5">
+        <f t="shared" ref="B105:M105" si="18">B92-B99</f>
+        <v>3.5386049700197875E-4</v>
+      </c>
+      <c r="C105" s="5">
+        <f t="shared" si="18"/>
+        <v>3.5378380091100059E-4</v>
+      </c>
+      <c r="D105" s="5">
+        <f t="shared" si="18"/>
+        <v>3.5309377756501115E-4</v>
+      </c>
+      <c r="E105" s="5">
+        <f t="shared" si="18"/>
+        <v>3.4621807503401603E-4</v>
+      </c>
+      <c r="F105" s="5">
+        <f t="shared" si="18"/>
+        <v>2.8066772829199449E-4</v>
+      </c>
+      <c r="G105" s="5">
+        <f t="shared" si="18"/>
+        <v>2.1624192714200796E-4</v>
+      </c>
+      <c r="H105" s="5">
+        <f t="shared" si="18"/>
+        <v>1.6078005812200646E-4</v>
+      </c>
+      <c r="I105" s="5">
+        <f t="shared" si="18"/>
+        <v>1.0849903958598528E-4</v>
+      </c>
+      <c r="J105" s="5">
+        <f t="shared" si="18"/>
+        <v>3.5300835807994257E-5</v>
+      </c>
+      <c r="K105" s="5">
+        <f t="shared" si="18"/>
+        <v>-8.8871770931003846E-5</v>
+      </c>
+      <c r="L105" s="5">
+        <f t="shared" si="18"/>
+        <v>-3.389762181350009E-4</v>
+      </c>
+      <c r="M105" s="5">
+        <f t="shared" si="18"/>
+        <v>-9.238067401129979E-4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="19">
+    <mergeCell ref="B93:M93"/>
+    <mergeCell ref="B100:M100"/>
+    <mergeCell ref="B65:M65"/>
+    <mergeCell ref="B72:M72"/>
+    <mergeCell ref="B79:M79"/>
+    <mergeCell ref="N80:R84"/>
+    <mergeCell ref="B86:M86"/>
     <mergeCell ref="N59:R63"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:M2"/>
@@ -6356,4 +8646,42 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>